<commit_message>
changed paystub data, progress on paystub
</commit_message>
<xml_diff>
--- a/data/tables/chart_of_accounts.xlsx
+++ b/data/tables/chart_of_accounts.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab5093ebb450c182/Python/Projects/financialstatements/financialstatements/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{8CFE3340-A4AF-4E24-B12F-F9390CE8BF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C3DA1B-400D-427F-AEAD-DC86B0D89FC2}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{8CFE3340-A4AF-4E24-B12F-F9390CE8BF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CCEE6D8-0585-419F-BD54-46FB40232810}"/>
   <bookViews>
-    <workbookView xWindow="-25845" yWindow="855" windowWidth="24270" windowHeight="12915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="2985" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chart_of_accounts" sheetId="2" r:id="rId1"/>
     <sheet name="mcc_list" sheetId="3" r:id="rId2"/>
     <sheet name="coa_mcc_link_table" sheetId="4" r:id="rId3"/>
+    <sheet name="coa_paystub_link_table" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">coa_mcc_link_table!$A$1:$D$1</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="1068">
   <si>
     <t>GL_Code</t>
   </si>
@@ -3176,6 +3177,72 @@
   </si>
   <si>
     <t>PAYMENT THANK YOU</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>INS MED U *</t>
+  </si>
+  <si>
+    <t>INS DEN U *</t>
+  </si>
+  <si>
+    <t>ROTH 401K</t>
+  </si>
+  <si>
+    <t>HSA CONTR *</t>
+  </si>
+  <si>
+    <t>CO STK CONT</t>
+  </si>
+  <si>
+    <t>STOCK PURCH</t>
+  </si>
+  <si>
+    <t>INS VIS *</t>
+  </si>
+  <si>
+    <t>EQUITY P/O NET</t>
+  </si>
+  <si>
+    <t>HEALTH CLUB</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>CO STK</t>
+  </si>
+  <si>
+    <t>FEDERAL TAX</t>
+  </si>
+  <si>
+    <t>SOCIAL SECURITY</t>
+  </si>
+  <si>
+    <t>MEDICARE</t>
+  </si>
+  <si>
+    <t>ARKANSAS</t>
+  </si>
+  <si>
+    <t>MTD AWARD</t>
+  </si>
+  <si>
+    <t>RS/RSU</t>
+  </si>
+  <si>
+    <t>MGMT</t>
+  </si>
+  <si>
+    <t>Making A Difference Reward</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Walton Life Fitness Center</t>
   </si>
 </sst>
 </file>
@@ -3780,10 +3847,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}" name="Chart_of_Accounts" displayName="Chart_of_Accounts" ref="A1:D70" totalsRowShown="0">
-  <autoFilter ref="A1:D70" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D70">
-    <sortCondition ref="A1:A70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}" name="Chart_of_Accounts" displayName="Chart_of_Accounts" ref="A1:D72" totalsRowShown="0">
+  <autoFilter ref="A1:D72" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
+    <sortCondition ref="A1:A72"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{9F7328E0-03C7-4074-9A0F-E8A9777A8A7D}" name="GL_Code"/>
@@ -4103,10 +4170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4441,24 +4508,24 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>500101</v>
+        <v>400104</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>1065</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>500102</v>
+        <v>500101</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
@@ -4469,10 +4536,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>500103</v>
+        <v>500102</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -4483,13 +4550,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>500201</v>
+        <v>500103</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
         <v>38</v>
@@ -4497,13 +4564,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>500202</v>
+        <v>500104</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>1067</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>1066</v>
       </c>
       <c r="D28" t="s">
         <v>38</v>
@@ -4511,10 +4578,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>500203</v>
+        <v>500201</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>42</v>
@@ -4525,10 +4592,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>500204</v>
+        <v>500202</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
         <v>42</v>
@@ -4539,13 +4606,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>500301</v>
+        <v>500203</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
         <v>38</v>
@@ -4553,41 +4620,41 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>600101</v>
+        <v>500204</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>600201</v>
+        <v>500301</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>600202</v>
+        <v>600101</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
         <v>49</v>
@@ -4595,13 +4662,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>600301</v>
+        <v>600201</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D35" t="s">
         <v>49</v>
@@ -4609,13 +4676,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>600401</v>
+        <v>600202</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
         <v>49</v>
@@ -4623,13 +4690,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>600501</v>
+        <v>600301</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
         <v>49</v>
@@ -4637,13 +4704,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>600502</v>
+        <v>600401</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
         <v>49</v>
@@ -4651,10 +4718,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>600503</v>
+        <v>600501</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>56</v>
@@ -4665,13 +4732,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>600601</v>
+        <v>600502</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
         <v>49</v>
@@ -4679,13 +4746,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>600602</v>
+        <v>600503</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
         <v>49</v>
@@ -4693,10 +4760,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>600603</v>
+        <v>600601</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
         <v>60</v>
@@ -4707,10 +4774,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>600604</v>
+        <v>600602</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
         <v>60</v>
@@ -4721,10 +4788,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>600605</v>
+        <v>600603</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
         <v>60</v>
@@ -4735,10 +4802,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>600606</v>
+        <v>600604</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
         <v>60</v>
@@ -4749,10 +4816,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>600607</v>
+        <v>600605</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>60</v>
@@ -4763,13 +4830,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>600701</v>
+        <v>600606</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -4777,13 +4844,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>600801</v>
+        <v>600607</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
         <v>49</v>
@@ -4791,13 +4858,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>600802</v>
+        <v>600701</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D49" t="s">
         <v>49</v>
@@ -4805,10 +4872,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>600803</v>
+        <v>600801</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
         <v>69</v>
@@ -4819,13 +4886,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>600901</v>
+        <v>600802</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
         <v>49</v>
@@ -4833,13 +4900,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>601001</v>
+        <v>600803</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D52" t="s">
         <v>49</v>
@@ -4847,13 +4914,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>601002</v>
+        <v>600901</v>
       </c>
       <c r="B53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
         <v>49</v>
@@ -4861,10 +4928,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>601003</v>
+        <v>601001</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
         <v>74</v>
@@ -4875,10 +4942,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>601004</v>
+        <v>601002</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
         <v>74</v>
@@ -4889,10 +4956,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>601005</v>
+        <v>601003</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
         <v>74</v>
@@ -4903,10 +4970,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>601006</v>
+        <v>601004</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
         <v>74</v>
@@ -4917,10 +4984,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>601007</v>
+        <v>601005</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
         <v>74</v>
@@ -4931,10 +4998,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>601008</v>
+        <v>601006</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
         <v>74</v>
@@ -4945,10 +5012,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>601009</v>
+        <v>601007</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
         <v>74</v>
@@ -4959,10 +5026,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>601010</v>
+        <v>601008</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
         <v>74</v>
@@ -4973,10 +5040,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>601011</v>
+        <v>601009</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
         <v>74</v>
@@ -4987,12 +5054,12 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>601012</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="2" t="s">
+        <v>601010</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" t="s">
         <v>74</v>
       </c>
       <c r="D63" t="s">
@@ -5001,12 +5068,12 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>601013</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C64" s="1" t="s">
+        <v>601011</v>
+      </c>
+      <c r="B64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" t="s">
         <v>74</v>
       </c>
       <c r="D64" t="s">
@@ -5015,12 +5082,12 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>601014</v>
-      </c>
-      <c r="B65" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" t="s">
+        <v>601012</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D65" t="s">
@@ -5029,12 +5096,12 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>601015</v>
-      </c>
-      <c r="B66" t="s">
-        <v>88</v>
-      </c>
-      <c r="C66" t="s">
+        <v>601013</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D66" t="s">
@@ -5043,10 +5110,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>601016</v>
+        <v>601014</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
         <v>74</v>
@@ -5057,10 +5124,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>601017</v>
+        <v>601015</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C68" t="s">
         <v>74</v>
@@ -5071,10 +5138,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>601018</v>
+        <v>601016</v>
       </c>
       <c r="B69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
         <v>74</v>
@@ -5085,10 +5152,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>601019</v>
+        <v>601017</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
         <v>74</v>
@@ -5097,9 +5164,37 @@
         <v>49</v>
       </c>
     </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>601018</v>
+      </c>
+      <c r="B71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>601019</v>
+      </c>
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E51:E70">
+  <conditionalFormatting sqref="E53:E72">
     <cfRule type="duplicateValues" dxfId="2" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13394,4 +13489,326 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC21C10-85DB-491C-9747-D63253F4E77A}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B2">
+        <v>400101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B3">
+        <v>400103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B4">
+        <v>400104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B5">
+        <v>100302</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B6">
+        <v>400102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B7">
+        <v>500201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B8">
+        <v>500202</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B9">
+        <v>500203</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B10">
+        <v>500204</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B11">
+        <v>500101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B12">
+        <v>500102</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B13">
+        <v>500103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B14">
+        <v>100305</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B15">
+        <v>100304</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B17">
+        <v>100202</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B19">
+        <v>500104</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to remove month table
</commit_message>
<xml_diff>
--- a/data/tables/chart_of_accounts.xlsx
+++ b/data/tables/chart_of_accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab5093ebb450c182/Python/Projects/financialstatements/financialstatements/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{8CFE3340-A4AF-4E24-B12F-F9390CE8BF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{564F8E09-395A-4A70-84BB-AAB78FD11CF3}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{8CFE3340-A4AF-4E24-B12F-F9390CE8BF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A8CDA5-034D-4722-89F0-1D194D6861D4}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="3045" windowWidth="28800" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chart_of_accounts" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="1078">
   <si>
     <t>GL_Code</t>
   </si>
@@ -3247,6 +3247,33 @@
   </si>
   <si>
     <t>Order_Col</t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Temporary</t>
+  </si>
+  <si>
+    <t>DEBIT</t>
+  </si>
+  <si>
+    <t>Natural_Balance</t>
+  </si>
+  <si>
+    <t>CREDIT</t>
+  </si>
+  <si>
+    <t>Retained Earnings</t>
+  </si>
+  <si>
+    <t>Net Income</t>
+  </si>
+  <si>
+    <t>Profit</t>
   </si>
 </sst>
 </file>
@@ -3395,7 +3422,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3575,14 +3602,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -3697,17 +3718,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3753,10 +3763,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3847,16 +3855,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}" name="Chart_of_Accounts" displayName="Chart_of_Accounts" ref="A1:D72" totalsRowShown="0">
-  <autoFilter ref="A1:D72" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
-    <sortCondition ref="A1:A72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}" name="Chart_of_Accounts" displayName="Chart_of_Accounts" ref="A1:F74" totalsRowShown="0">
+  <autoFilter ref="A1:F74" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
+    <sortCondition ref="A1:A73"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{9F7328E0-03C7-4074-9A0F-E8A9777A8A7D}" name="GL_Code"/>
     <tableColumn id="3" xr3:uid="{2E834F2B-4EAF-4EE4-9503-61683A98D5B5}" name="Account"/>
     <tableColumn id="7" xr3:uid="{FA5AFEA8-C5E7-4AA3-9924-05C97BDC6FF7}" name="Category"/>
     <tableColumn id="5" xr3:uid="{848C2A2A-2CF6-42CD-8423-EAFD72FB3EBC}" name="Account_Type"/>
+    <tableColumn id="1" xr3:uid="{1FBE17F8-413D-461A-B7BF-2BCD38A11314}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{709F292D-88A0-460F-BC4A-3A8DE4FDBB01}" name="Natural_Balance"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4170,10 +4180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4182,9 +4192,10 @@
     <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4197,8 +4208,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100101</v>
       </c>
@@ -4211,8 +4228,14 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100102</v>
       </c>
@@ -4225,8 +4248,14 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100103</v>
       </c>
@@ -4239,8 +4268,14 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100201</v>
       </c>
@@ -4253,8 +4288,14 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100202</v>
       </c>
@@ -4267,8 +4308,14 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>100203</v>
       </c>
@@ -4281,8 +4328,14 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100204</v>
       </c>
@@ -4295,8 +4348,14 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>100301</v>
       </c>
@@ -4309,8 +4368,14 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>100302</v>
       </c>
@@ -4323,8 +4388,14 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100303</v>
       </c>
@@ -4337,8 +4408,14 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100304</v>
       </c>
@@ -4351,8 +4428,14 @@
       <c r="D12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>100305</v>
       </c>
@@ -4365,8 +4448,14 @@
       <c r="D13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>100401</v>
       </c>
@@ -4379,8 +4468,14 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>100402</v>
       </c>
@@ -4393,8 +4488,14 @@
       <c r="D15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>100403</v>
       </c>
@@ -4407,8 +4508,14 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>100404</v>
       </c>
@@ -4421,8 +4528,14 @@
       <c r="D17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>100405</v>
       </c>
@@ -4435,8 +4548,14 @@
       <c r="D18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>200101</v>
       </c>
@@ -4449,8 +4568,14 @@
       <c r="D19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>300101</v>
       </c>
@@ -4463,27 +4588,39 @@
       <c r="D20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>300102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>400101</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>31</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>400102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -4491,13 +4628,19 @@
       <c r="D22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>400103</v>
+        <v>400102</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -4505,13 +4648,19 @@
       <c r="D23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>400104</v>
+        <v>400103</v>
       </c>
       <c r="B24" t="s">
-        <v>1065</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -4519,27 +4668,39 @@
       <c r="D24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>400104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>500101</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>500102</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -4547,13 +4708,19 @@
       <c r="D26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>500103</v>
+        <v>500102</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
@@ -4561,41 +4728,59 @@
       <c r="D27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>500104</v>
+        <v>500103</v>
       </c>
       <c r="B28" t="s">
-        <v>1067</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>1066</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>500201</v>
+        <v>500104</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>1067</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>1066</v>
       </c>
       <c r="D29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>500202</v>
+        <v>500201</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
         <v>42</v>
@@ -4603,13 +4788,19 @@
       <c r="D30" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>500203</v>
+        <v>500202</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>42</v>
@@ -4617,13 +4808,19 @@
       <c r="D31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>500204</v>
+        <v>500203</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
         <v>42</v>
@@ -4631,55 +4828,79 @@
       <c r="D32" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>500301</v>
+        <v>500204</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
+        <v>500301</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>600101</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>47</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>48</v>
-      </c>
-      <c r="D34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>600201</v>
-      </c>
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" t="s">
-        <v>51</v>
       </c>
       <c r="D35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>600202</v>
+        <v>600201</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
         <v>51</v>
@@ -4687,55 +4908,79 @@
       <c r="D36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>600301</v>
+        <v>600202</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>600401</v>
+        <v>600301</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>600501</v>
+        <v>600401</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>600502</v>
+        <v>600501</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
         <v>56</v>
@@ -4743,13 +4988,19 @@
       <c r="D40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>600503</v>
+        <v>600502</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
         <v>56</v>
@@ -4757,27 +5008,39 @@
       <c r="D41" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>600601</v>
+        <v>600503</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>600602</v>
+        <v>600601</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
         <v>60</v>
@@ -4785,13 +5048,19 @@
       <c r="D43" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>600603</v>
+        <v>600602</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
         <v>60</v>
@@ -4799,13 +5068,19 @@
       <c r="D44" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>600604</v>
+        <v>600603</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
         <v>60</v>
@@ -4813,13 +5088,19 @@
       <c r="D45" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>600605</v>
+        <v>600604</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
         <v>60</v>
@@ -4827,13 +5108,19 @@
       <c r="D46" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>600606</v>
+        <v>600605</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
         <v>60</v>
@@ -4841,13 +5128,19 @@
       <c r="D47" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>600607</v>
+        <v>600606</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
         <v>60</v>
@@ -4855,41 +5148,59 @@
       <c r="D48" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>600701</v>
+        <v>600607</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>600801</v>
+        <v>600701</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>600802</v>
+        <v>600801</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
         <v>69</v>
@@ -4897,13 +5208,19 @@
       <c r="D51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>600803</v>
+        <v>600802</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
         <v>69</v>
@@ -4911,41 +5228,59 @@
       <c r="D52" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>600901</v>
+        <v>600803</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>601001</v>
+        <v>600901</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="D54" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>601002</v>
+        <v>601001</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
         <v>74</v>
@@ -4953,13 +5288,19 @@
       <c r="D55" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>601003</v>
+        <v>601002</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
         <v>74</v>
@@ -4967,13 +5308,19 @@
       <c r="D56" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>601004</v>
+        <v>601003</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
         <v>74</v>
@@ -4981,13 +5328,19 @@
       <c r="D57" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>601005</v>
+        <v>601004</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
         <v>74</v>
@@ -4995,13 +5348,19 @@
       <c r="D58" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>601006</v>
+        <v>601005</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
         <v>74</v>
@@ -5009,13 +5368,19 @@
       <c r="D59" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>601007</v>
+        <v>601006</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
         <v>74</v>
@@ -5023,13 +5388,19 @@
       <c r="D60" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>601008</v>
+        <v>601007</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" t="s">
         <v>74</v>
@@ -5037,13 +5408,19 @@
       <c r="D61" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>601009</v>
+        <v>601008</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
         <v>74</v>
@@ -5051,13 +5428,19 @@
       <c r="D62" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>601010</v>
+        <v>601009</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
         <v>74</v>
@@ -5065,13 +5448,19 @@
       <c r="D63" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>601011</v>
+        <v>601010</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
         <v>74</v>
@@ -5079,41 +5468,59 @@
       <c r="D64" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>601012</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="2" t="s">
+        <v>601011</v>
+      </c>
+      <c r="B65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" t="s">
         <v>74</v>
       </c>
       <c r="D65" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>601013</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C66" s="1" t="s">
+        <v>601012</v>
+      </c>
+      <c r="B66" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" t="s">
         <v>74</v>
       </c>
       <c r="D66" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>601014</v>
+        <v>601013</v>
       </c>
       <c r="B67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
         <v>74</v>
@@ -5121,13 +5528,19 @@
       <c r="D67" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>601015</v>
+        <v>601014</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
         <v>74</v>
@@ -5135,13 +5548,19 @@
       <c r="D68" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>601016</v>
+        <v>601015</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
         <v>74</v>
@@ -5149,13 +5568,19 @@
       <c r="D69" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>601017</v>
+        <v>601016</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
         <v>74</v>
@@ -5163,13 +5588,19 @@
       <c r="D70" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>601018</v>
+        <v>601017</v>
       </c>
       <c r="B71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C71" t="s">
         <v>74</v>
@@ -5177,13 +5608,19 @@
       <c r="D71" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>601019</v>
+        <v>601018</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C72" t="s">
         <v>74</v>
@@ -5191,12 +5628,55 @@
       <c r="D72" t="s">
         <v>49</v>
       </c>
+      <c r="E72" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>601019</v>
+      </c>
+      <c r="B73" t="s">
+        <v>92</v>
+      </c>
+      <c r="C73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>700001</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1074</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E53:E72">
-    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Starting income statement dev
</commit_message>
<xml_diff>
--- a/data/tables/chart_of_accounts.xlsx
+++ b/data/tables/chart_of_accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab5093ebb450c182/Python/Projects/financialstatements/financialstatements/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{8CFE3340-A4AF-4E24-B12F-F9390CE8BF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A8CDA5-034D-4722-89F0-1D194D6861D4}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{8CFE3340-A4AF-4E24-B12F-F9390CE8BF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1FE87C6-B5EB-4B68-BAED-3366F75A2F6A}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="3045" windowWidth="28800" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="2145" windowWidth="28800" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chart_of_accounts" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1079">
   <si>
     <t>GL_Code</t>
   </si>
@@ -3252,18 +3252,12 @@
     <t>Permanent</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Temporary</t>
   </si>
   <si>
     <t>DEBIT</t>
   </si>
   <si>
-    <t>Natural_Balance</t>
-  </si>
-  <si>
     <t>CREDIT</t>
   </si>
   <si>
@@ -3274,6 +3268,15 @@
   </si>
   <si>
     <t>Profit</t>
+  </si>
+  <si>
+    <t>Income after Deductions and Taxes</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Account_Classification</t>
   </si>
 </sst>
 </file>
@@ -3810,17 +3813,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3854,9 +3847,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}" name="Chart_of_Accounts" displayName="Chart_of_Accounts" ref="A1:F74" totalsRowShown="0">
-  <autoFilter ref="A1:F74" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}" name="Chart_of_Accounts" displayName="Chart_of_Accounts" ref="A1:F75" totalsRowShown="0">
+  <autoFilter ref="A1:F75" xr:uid="{77394BDD-A871-4C4C-8335-72F962419DC6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
     <sortCondition ref="A1:A73"/>
   </sortState>
@@ -3865,8 +3862,8 @@
     <tableColumn id="3" xr3:uid="{2E834F2B-4EAF-4EE4-9503-61683A98D5B5}" name="Account"/>
     <tableColumn id="7" xr3:uid="{FA5AFEA8-C5E7-4AA3-9924-05C97BDC6FF7}" name="Category"/>
     <tableColumn id="5" xr3:uid="{848C2A2A-2CF6-42CD-8423-EAFD72FB3EBC}" name="Account_Type"/>
-    <tableColumn id="1" xr3:uid="{1FBE17F8-413D-461A-B7BF-2BCD38A11314}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{709F292D-88A0-460F-BC4A-3A8DE4FDBB01}" name="Natural_Balance"/>
+    <tableColumn id="1" xr3:uid="{1FBE17F8-413D-461A-B7BF-2BCD38A11314}" name="Account_Classification"/>
+    <tableColumn id="2" xr3:uid="{709F292D-88A0-460F-BC4A-3A8DE4FDBB01}" name="Nature"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4180,10 +4177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4191,7 +4188,8 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4209,10 +4207,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>1070</v>
+        <v>1078</v>
       </c>
       <c r="F1" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4232,7 +4230,7 @@
         <v>1069</v>
       </c>
       <c r="F2" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4252,7 +4250,7 @@
         <v>1069</v>
       </c>
       <c r="F3" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4272,7 +4270,7 @@
         <v>1069</v>
       </c>
       <c r="F4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4292,7 +4290,7 @@
         <v>1069</v>
       </c>
       <c r="F5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4312,7 +4310,7 @@
         <v>1069</v>
       </c>
       <c r="F6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4332,7 +4330,7 @@
         <v>1069</v>
       </c>
       <c r="F7" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4352,7 +4350,7 @@
         <v>1069</v>
       </c>
       <c r="F8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4372,7 +4370,7 @@
         <v>1069</v>
       </c>
       <c r="F9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4392,7 +4390,7 @@
         <v>1069</v>
       </c>
       <c r="F10" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4412,7 +4410,7 @@
         <v>1069</v>
       </c>
       <c r="F11" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4432,7 +4430,7 @@
         <v>1069</v>
       </c>
       <c r="F12" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4452,7 +4450,7 @@
         <v>1069</v>
       </c>
       <c r="F13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4472,7 +4470,7 @@
         <v>1069</v>
       </c>
       <c r="F14" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4492,7 +4490,7 @@
         <v>1069</v>
       </c>
       <c r="F15" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4512,7 +4510,7 @@
         <v>1069</v>
       </c>
       <c r="F16" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4532,7 +4530,7 @@
         <v>1069</v>
       </c>
       <c r="F17" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4552,7 +4550,7 @@
         <v>1069</v>
       </c>
       <c r="F18" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4572,7 +4570,7 @@
         <v>1069</v>
       </c>
       <c r="F19" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4592,7 +4590,7 @@
         <v>1069</v>
       </c>
       <c r="F20" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4600,7 +4598,7 @@
         <v>300102</v>
       </c>
       <c r="B21" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -4612,7 +4610,7 @@
         <v>1069</v>
       </c>
       <c r="F21" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4629,10 +4627,10 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F22" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4649,10 +4647,10 @@
         <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4669,10 +4667,10 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F24" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4689,10 +4687,10 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F25" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4709,10 +4707,10 @@
         <v>38</v>
       </c>
       <c r="E26" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F26" t="s">
         <v>1071</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4729,10 +4727,10 @@
         <v>38</v>
       </c>
       <c r="E27" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F27" t="s">
         <v>1071</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4749,10 +4747,10 @@
         <v>38</v>
       </c>
       <c r="E28" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F28" t="s">
         <v>1071</v>
-      </c>
-      <c r="F28" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4769,10 +4767,10 @@
         <v>38</v>
       </c>
       <c r="E29" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F29" t="s">
         <v>1071</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4789,10 +4787,10 @@
         <v>38</v>
       </c>
       <c r="E30" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F30" t="s">
         <v>1071</v>
-      </c>
-      <c r="F30" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4809,10 +4807,10 @@
         <v>38</v>
       </c>
       <c r="E31" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F31" t="s">
         <v>1071</v>
-      </c>
-      <c r="F31" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4829,10 +4827,10 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F32" t="s">
         <v>1071</v>
-      </c>
-      <c r="F32" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4849,10 +4847,10 @@
         <v>38</v>
       </c>
       <c r="E33" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F33" t="s">
         <v>1071</v>
-      </c>
-      <c r="F33" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4869,10 +4867,10 @@
         <v>38</v>
       </c>
       <c r="E34" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F34" t="s">
         <v>1071</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4889,10 +4887,10 @@
         <v>49</v>
       </c>
       <c r="E35" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F35" t="s">
         <v>1071</v>
-      </c>
-      <c r="F35" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4909,10 +4907,10 @@
         <v>49</v>
       </c>
       <c r="E36" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F36" t="s">
         <v>1071</v>
-      </c>
-      <c r="F36" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4929,10 +4927,10 @@
         <v>49</v>
       </c>
       <c r="E37" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F37" t="s">
         <v>1071</v>
-      </c>
-      <c r="F37" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4949,10 +4947,10 @@
         <v>49</v>
       </c>
       <c r="E38" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F38" t="s">
         <v>1071</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4969,10 +4967,10 @@
         <v>49</v>
       </c>
       <c r="E39" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F39" t="s">
         <v>1071</v>
-      </c>
-      <c r="F39" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4989,10 +4987,10 @@
         <v>49</v>
       </c>
       <c r="E40" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F40" t="s">
         <v>1071</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -5009,10 +5007,10 @@
         <v>49</v>
       </c>
       <c r="E41" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F41" t="s">
         <v>1071</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -5029,10 +5027,10 @@
         <v>49</v>
       </c>
       <c r="E42" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F42" t="s">
         <v>1071</v>
-      </c>
-      <c r="F42" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -5049,10 +5047,10 @@
         <v>49</v>
       </c>
       <c r="E43" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F43" t="s">
         <v>1071</v>
-      </c>
-      <c r="F43" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5069,10 +5067,10 @@
         <v>49</v>
       </c>
       <c r="E44" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F44" t="s">
         <v>1071</v>
-      </c>
-      <c r="F44" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -5089,10 +5087,10 @@
         <v>49</v>
       </c>
       <c r="E45" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F45" t="s">
         <v>1071</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -5109,10 +5107,10 @@
         <v>49</v>
       </c>
       <c r="E46" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F46" t="s">
         <v>1071</v>
-      </c>
-      <c r="F46" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5129,10 +5127,10 @@
         <v>49</v>
       </c>
       <c r="E47" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F47" t="s">
         <v>1071</v>
-      </c>
-      <c r="F47" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -5149,10 +5147,10 @@
         <v>49</v>
       </c>
       <c r="E48" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F48" t="s">
         <v>1071</v>
-      </c>
-      <c r="F48" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5169,10 +5167,10 @@
         <v>49</v>
       </c>
       <c r="E49" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F49" t="s">
         <v>1071</v>
-      </c>
-      <c r="F49" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5189,10 +5187,10 @@
         <v>49</v>
       </c>
       <c r="E50" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F50" t="s">
         <v>1071</v>
-      </c>
-      <c r="F50" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -5209,10 +5207,10 @@
         <v>49</v>
       </c>
       <c r="E51" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F51" t="s">
         <v>1071</v>
-      </c>
-      <c r="F51" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -5229,10 +5227,10 @@
         <v>49</v>
       </c>
       <c r="E52" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F52" t="s">
         <v>1071</v>
-      </c>
-      <c r="F52" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -5249,10 +5247,10 @@
         <v>49</v>
       </c>
       <c r="E53" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F53" t="s">
         <v>1071</v>
-      </c>
-      <c r="F53" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -5269,10 +5267,10 @@
         <v>49</v>
       </c>
       <c r="E54" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F54" t="s">
         <v>1071</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -5289,10 +5287,10 @@
         <v>49</v>
       </c>
       <c r="E55" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F55" t="s">
         <v>1071</v>
-      </c>
-      <c r="F55" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -5309,10 +5307,10 @@
         <v>49</v>
       </c>
       <c r="E56" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F56" t="s">
         <v>1071</v>
-      </c>
-      <c r="F56" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -5329,10 +5327,10 @@
         <v>49</v>
       </c>
       <c r="E57" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F57" t="s">
         <v>1071</v>
-      </c>
-      <c r="F57" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5349,10 +5347,10 @@
         <v>49</v>
       </c>
       <c r="E58" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F58" t="s">
         <v>1071</v>
-      </c>
-      <c r="F58" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5369,10 +5367,10 @@
         <v>49</v>
       </c>
       <c r="E59" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F59" t="s">
         <v>1071</v>
-      </c>
-      <c r="F59" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5389,10 +5387,10 @@
         <v>49</v>
       </c>
       <c r="E60" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F60" t="s">
         <v>1071</v>
-      </c>
-      <c r="F60" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5409,10 +5407,10 @@
         <v>49</v>
       </c>
       <c r="E61" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F61" t="s">
         <v>1071</v>
-      </c>
-      <c r="F61" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5429,10 +5427,10 @@
         <v>49</v>
       </c>
       <c r="E62" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F62" t="s">
         <v>1071</v>
-      </c>
-      <c r="F62" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5449,10 +5447,10 @@
         <v>49</v>
       </c>
       <c r="E63" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F63" t="s">
         <v>1071</v>
-      </c>
-      <c r="F63" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5469,10 +5467,10 @@
         <v>49</v>
       </c>
       <c r="E64" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F64" t="s">
         <v>1071</v>
-      </c>
-      <c r="F64" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5489,10 +5487,10 @@
         <v>49</v>
       </c>
       <c r="E65" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F65" t="s">
         <v>1071</v>
-      </c>
-      <c r="F65" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5509,10 +5507,10 @@
         <v>49</v>
       </c>
       <c r="E66" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F66" t="s">
         <v>1071</v>
-      </c>
-      <c r="F66" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5529,10 +5527,10 @@
         <v>49</v>
       </c>
       <c r="E67" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F67" t="s">
         <v>1071</v>
-      </c>
-      <c r="F67" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -5549,10 +5547,10 @@
         <v>49</v>
       </c>
       <c r="E68" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F68" t="s">
         <v>1071</v>
-      </c>
-      <c r="F68" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5569,10 +5567,10 @@
         <v>49</v>
       </c>
       <c r="E69" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F69" t="s">
         <v>1071</v>
-      </c>
-      <c r="F69" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -5589,10 +5587,10 @@
         <v>49</v>
       </c>
       <c r="E70" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F70" t="s">
         <v>1071</v>
-      </c>
-      <c r="F70" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -5609,10 +5607,10 @@
         <v>49</v>
       </c>
       <c r="E71" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F71" t="s">
         <v>1071</v>
-      </c>
-      <c r="F71" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -5629,10 +5627,10 @@
         <v>49</v>
       </c>
       <c r="E72" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F72" t="s">
         <v>1071</v>
-      </c>
-      <c r="F72" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -5649,10 +5647,10 @@
         <v>49</v>
       </c>
       <c r="E73" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F73" t="s">
         <v>1071</v>
-      </c>
-      <c r="F73" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -5663,16 +5661,36 @@
         <v>1076</v>
       </c>
       <c r="C74" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D74" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="E74" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F74" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>700002</v>
+      </c>
+      <c r="B75" t="s">
         <v>1074</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>